<commit_message>
Updated Ticket_Analysis.xlsx with latest data
</commit_message>
<xml_diff>
--- a/Spreadsheets/Ticket_Analysis.xlsx
+++ b/Spreadsheets/Ticket_Analysis.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Data_Analyst_Assignment\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7BFD76-911D-4ACA-B897-DD28466680F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADE0F86-CAA0-4477-A37C-15B8D2F1B1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{101D4051-F827-4C33-AB08-9434B19B47F0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{101D4051-F827-4C33-AB08-9434B19B47F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="ticket" sheetId="1" r:id="rId1"/>
-    <sheet name="feedbacks" sheetId="2" r:id="rId2"/>
+    <sheet name="feedbacks" sheetId="2" r:id="rId1"/>
+    <sheet name="ticket" sheetId="1" r:id="rId2"/>
     <sheet name="Results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,6 +35,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
@@ -102,6 +124,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -144,11 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,6 +488,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DEACC8-EA2C-41DC-ADEF-E7EDD4D744C3}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <f>IFERROR(INDEX(ticket!$B$2:$B$1000, MATCH(A2, ticket!$E$2:$E$1000, 0)), "")</f>
+        <v>44429.560277777775</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44429.560277777775</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4">
+        <f>IFERROR(INDEX(ticket!$B$2:$B$1000, MATCH(A3, ticket!$E$2:$E$1000, 0)), "")</f>
+        <v>44430.375</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44430.416666666664</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D72CDA4-4C6C-46DD-B8F7-C55B80F959B1}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -565,69 +655,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DEACC8-EA2C-41DC-ADEF-E7EDD4D744C3}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2">
-        <v>44429.560277777775</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2">
-        <v>44430.416666666664</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB03EE4E-8E9E-45E6-8ED8-31C341AD2C38}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -651,10 +684,26 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" cm="1">
+        <f t="array" ref="B2">SUMPRODUCT((ticket!$D$2:$D$1000 = $A2) * (INT(ticket!$B$2:$B$1000) = INT(ticket!$C$2:$C$1000)))</f>
+        <v>3</v>
+      </c>
+      <c r="C2" cm="1">
+        <f t="array" ref="C2">SUMPRODUCT((ticket!$D$2:$D$1000 = $A2) * (INT(ticket!$B$2:$B$1000) = INT(ticket!$C$2:$C$1000)) * (HOUR(ticket!$B$2:$B$1000) = HOUR(ticket!$C$2:$C$1000)))</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>16</v>
+      </c>
+      <c r="B3" cm="1">
+        <f t="array" ref="B3">SUMPRODUCT((ticket!$D$2:$D$1000 = $A3) * (INT(ticket!$B$2:$B$1000) = INT(ticket!$C$2:$C$1000)))</f>
+        <v>1</v>
+      </c>
+      <c r="C3" cm="1">
+        <f t="array" ref="C3">SUMPRODUCT((ticket!$D$2:$D$1000 = $A3) * (INT(ticket!$B$2:$B$1000) = INT(ticket!$C$2:$C$1000)) * (HOUR(ticket!$B$2:$B$1000) = HOUR(ticket!$C$2:$C$1000)))</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>